<commit_message>
Improving SBML report, implementing Kwakros
</commit_message>
<xml_diff>
--- a/python/mysite/sim/sbml/annotation/examples/Koenig2014_demo_kinetic_v7_annotations.xlsx
+++ b/python/mysite/sim/sbml/annotation/examples/Koenig2014_demo_kinetic_v7_annotations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="797" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="631" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Annotations" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,14 +14,14 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Annotations!$B$1:$B$13</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Annotations!$B$1:$B$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Annotations!$B$1:$B$20</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="69">
   <si>
     <t>id</t>
   </si>
@@ -95,18 +95,30 @@
     <t>11</t>
   </si>
   <si>
+    <t>biomodels.sbo</t>
+  </si>
+  <si>
+    <t>SBO:0000011</t>
+  </si>
+  <si>
     <t>^Km_(.)+$</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
+    <t>SBO:0000012</t>
+  </si>
+  <si>
     <t>^Keq_(.)+$</t>
   </si>
   <si>
     <t>13</t>
   </si>
   <si>
+    <t>SBO:0000013</t>
+  </si>
+  <si>
     <t>types</t>
   </si>
   <si>
@@ -162,9 +174,6 @@
   </si>
   <si>
     <t>BQB_IS_HOMOLOG_TO</t>
-  </si>
-  <si>
-    <t>biomodels.sbo</t>
   </si>
   <si>
     <t>tcdb</t>
@@ -431,12 +440,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -620,17 +629,21 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>25</v>
       </c>
     </row>
@@ -650,18 +663,69 @@
         <v>27</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B1:B13"/>
-  <dataValidations count="5">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1:B13" type="list">
+  <dataValidations count="6">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1:B16" type="list">
       <formula1>Allowed_Values!$B$2:$B$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C13" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C16" type="list">
       <formula1>Allowed_Values!$A$2:$A$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D8" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D8 D12 D14 D16" type="list">
       <formula1>Allowed_Values!$C$2:$C$17</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -669,8 +733,12 @@
       <formula1>Allowed_Values!$D$2:$D$27</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E13" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E16" type="list">
       <formula1>Allowed_Values!$D$2:$D$27</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2" type="list">
+      <formula1>Allowed_Values!$D$2:$D$28</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -690,10 +758,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:27"/>
+  <dimension ref="1:28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -707,16 +775,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="0"/>
@@ -1747,7 +1815,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>10</v>
@@ -1761,10 +1829,10 @@
         <v>17</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,22 +1840,22 @@
         <v>7</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E5" s="6"/>
     </row>
@@ -1796,7 +1864,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>13</v>
@@ -1805,10 +1873,10 @@
     </row>
     <row r="7" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>15</v>
@@ -1817,28 +1885,28 @@
     </row>
     <row r="8" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="E10" s="6"/>
     </row>
@@ -1847,34 +1915,34 @@
         <v>14</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="9" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E14" s="6"/>
     </row>
@@ -1888,20 +1956,20 @@
     </row>
     <row r="16" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1916,37 +1984,42 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="6" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D28" s="9" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2002,22 +2075,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G1" s="0"/>
       <c r="H1" s="0"/>
@@ -3040,10 +3113,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -3052,10 +3125,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>

</xml_diff>